<commit_message>
project updated with plots
</commit_message>
<xml_diff>
--- a/Project/Data/Residual comparison.xlsx
+++ b/Project/Data/Residual comparison.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\ETH Zurich Fall 2021\Physical Human Robot Interaction\Physical-Human-Robot-Interaction-Lab\Project\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1288FA-E80E-4C3F-873F-3F67CB3F1847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="15315" windowHeight="6735"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>residual max</t>
   </si>
@@ -112,24 +118,35 @@
   </si>
   <si>
     <t>0.0302</t>
+  </si>
+  <si>
+    <t>R-square</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -159,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,19 +184,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -217,9 +254,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +288,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,9 +340,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,46 +533,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="B1" s="1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="5">
         <v>9</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1">
+      <c r="C1" s="5"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="5">
         <v>10</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5">
         <v>11</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5">
         <v>12</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5">
         <v>13</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -507,31 +582,34 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>0</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -541,32 +619,35 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="6">
+        <v>0.88519999999999999</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -576,32 +657,35 @@
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7">
+        <v>0.88419999999999999</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>22</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -611,64 +695,70 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="8">
+        <v>0.91390000000000005</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>